<commit_message>
updated gc - buffer
</commit_message>
<xml_diff>
--- a/alu-4/GatterEquivalente.xlsx
+++ b/alu-4/GatterEquivalente.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>Typ</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Multiplizierer</t>
+  </si>
+  <si>
+    <t>Buffer4</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -565,11 +568,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -674,6 +725,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1788,7 @@
         <v>20</v>
       </c>
       <c r="H20" s="18">
-        <f t="shared" si="2"/>
+        <f>SUM(I$2*I20,J$2*J20,K$2*K20,L$2*L20,M$2*M20,N$2*N20,O$2*O20,P$2*P20,R$2*R20,S$2*S20,T$2*T20,U$2*U20)</f>
         <v>21</v>
       </c>
       <c r="I20" s="33"/>
@@ -1972,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="8">
-        <f t="shared" ref="D27:D33" si="4">B27*C27</f>
+        <f t="shared" ref="D27:D34" si="4">B27*C27</f>
         <v>0</v>
       </c>
       <c r="G27" s="16" t="s">
@@ -2164,11 +2231,11 @@
       <c r="T32" s="36"/>
       <c r="U32" s="18"/>
     </row>
-    <row r="33" spans="1:26" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="41">
         <v>1</v>
       </c>
       <c r="C33" s="7">
@@ -2199,20 +2266,21 @@
       <c r="U33" s="18"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="25">
-        <f>SUM(K3)</f>
-        <v>108.5</v>
-      </c>
-      <c r="D34" s="13">
-        <f>SUM(D26:D33,D3:D24,C34)</f>
-        <v>711.5</v>
-      </c>
+      <c r="A34" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="44">
+        <v>4</v>
+      </c>
+      <c r="C34" s="27">
+        <f>H34</f>
+        <v>19</v>
+      </c>
+      <c r="D34" s="27">
+        <f>B34*C34</f>
+        <v>76</v>
+      </c>
+      <c r="E34" s="42"/>
       <c r="G34" s="17" t="s">
         <v>43</v>
       </c>
@@ -2244,7 +2312,21 @@
       <c r="T34" s="36"/>
       <c r="U34" s="18"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="43">
+        <f>SUM(K3)</f>
+        <v>108.5</v>
+      </c>
+      <c r="D35" s="13">
+        <f>SUM(D26:D34,D3:D24,C35)</f>
+        <v>787.5</v>
+      </c>
       <c r="G35" s="17" t="s">
         <v>47</v>
       </c>

</xml_diff>